<commit_message>
Added non-mean centered body awareness
This means all data files are updated. Frequentist analysis code is also updated
</commit_message>
<xml_diff>
--- a/data/codebooks/MSC_codebook_processed.xlsx
+++ b/data/codebooks/MSC_codebook_processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncole\Documents\GitHub\ManySmilesCollaboration\data\codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Coles work\Documents\GitHub\data\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED059A40-234B-44C8-89A6-B624A2023D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3F7560-416F-4061-AA3E-B74BD4CD86AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1605" windowWidth="25380" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DF.l.inc" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="103">
   <si>
     <t>ResponseId</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>Report of how difficult participant found the movement task</t>
+  </si>
+  <si>
+    <t>indiv_body.c</t>
+  </si>
+  <si>
+    <t>indiv_body mean centered</t>
   </si>
 </sst>
 </file>
@@ -1284,21 +1290,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1327,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1332,7 +1338,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="166.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>96</v>
       </c>
@@ -1531,7 +1537,7 @@
       </c>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1559,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1564,7 +1570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1608,7 +1614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1641,7 +1647,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1667,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1670,7 +1676,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1679,7 +1685,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="93" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1716,7 @@
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
@@ -1718,6 +1724,14 @@
         <v>95</v>
       </c>
       <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>